<commit_message>
versão final - animação
</commit_message>
<xml_diff>
--- a/ExercícioHomogenea.xlsx
+++ b/ExercícioHomogenea.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e\phd_coder\Documents\Facul\CG\cg2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32B6DBB-CE34-4EC3-BFDD-939EA7139701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724C1354-FA31-4C4D-990C-577AD720D6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{71A544FD-4658-4102-90A6-8C668B312ACF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">ponto central </t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Matriz de de-translação</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
   </si>
 </sst>
 </file>
@@ -514,15 +523,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23817C73-DC59-4F06-AA22-33B4C71B7037}">
-  <dimension ref="B1:K16"/>
+  <dimension ref="B1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -530,12 +539,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -561,8 +570,17 @@
       <c r="K3">
         <v>-10</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>0</v>
       </c>
@@ -587,8 +605,21 @@
       <c r="K4">
         <v>-6</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>-2.5</v>
+      </c>
+      <c r="O4">
+        <v>-2.5</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <f>AVERAGE(N4:P4)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>0</v>
       </c>
@@ -613,8 +644,15 @@
       <c r="K5">
         <v>-4</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q6" si="0">AVERAGE(N5:P5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>0</v>
       </c>
@@ -639,13 +677,26 @@
       <c r="K6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>-2.5</v>
+      </c>
+      <c r="O6">
+        <v>2.5</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>3</v>
       </c>
@@ -666,7 +717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>0</v>
       </c>
@@ -686,7 +737,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>0</v>
       </c>
@@ -706,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>0</v>
       </c>
@@ -726,12 +777,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>1</v>
       </c>
@@ -757,7 +808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>0</v>
       </c>
@@ -783,7 +834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>0</v>
       </c>
@@ -809,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>0</v>
       </c>

</xml_diff>